<commit_message>
inclusao de preco fertilizando INDEX_MUNDI
</commit_message>
<xml_diff>
--- a/dataset/World_Bank-Population_oil_query.xlsx
+++ b/dataset/World_Bank-Population_oil_query.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projetos\vegetable_oil_mkt\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F52FDC2-FDE4-46D5-AA2F-0E2B4D8A5832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B685A4F5-8FB2-403B-8ED6-C48A468F6333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Series - Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AI$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Data!$A$1:$AI$337</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1001,13 +1001,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AI341"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="AH316" sqref="AH316"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,7 +1139,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1245,7 +1246,7 @@
         <v>17.149364497767507</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -1352,7 +1353,7 @@
         <v>68621946104.186455</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>165</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>3386420411905.0977</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>165</v>
       </c>
@@ -1566,7 +1567,7 @@
         <v>-5.706189649381102</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -1673,7 +1674,7 @@
         <v>1834.9134625163647</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -1780,7 +1781,7 @@
         <v>6094.6335084232742</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -1887,7 +1888,7 @@
         <v>11317017708430.697</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -1994,7 +1995,7 @@
         <v>4.350723509404915</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>165</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>69.867846801550968</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>165</v>
       </c>
@@ -2208,7 +2209,7 @@
         <v>38.5</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>165</v>
       </c>
@@ -2315,7 +2316,7 @@
         <v>6133.0365220334443</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>165</v>
       </c>
@@ -2422,7 +2423,7 @@
         <v>11388327588587.188</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>165</v>
       </c>
@@ -2529,7 +2530,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>165</v>
       </c>
@@ -2636,7 +2637,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>165</v>
       </c>
@@ -2743,7 +2744,7 @@
         <v>4770754</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>165</v>
       </c>
@@ -2850,7 +2851,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>165</v>
       </c>
@@ -2957,7 +2958,7 @@
         <v>1856882402</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>165</v>
       </c>
@@ -3064,7 +3065,7 @@
         <v>898262751</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>165</v>
       </c>
@@ -3171,7 +3172,7 @@
         <v>1.1496840659715417</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>165</v>
       </c>
@@ -3385,7 +3386,7 @@
         <v>1627.4989249753448</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -3492,7 +3493,7 @@
         <v>20.015022260283271</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -3599,7 +3600,7 @@
         <v>30149755796.564922</v>
       </c>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -3706,7 +3707,7 @@
         <v>1705379934850.6116</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>63</v>
       </c>
@@ -3813,7 +3814,7 @@
         <v>-2.0121354065442745</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -3920,7 +3921,7 @@
         <v>1506.5013936964206</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>63</v>
       </c>
@@ -4027,7 +4028,7 @@
         <v>3795.4314878852501</v>
       </c>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -4134,7 +4135,7 @@
         <v>4311787701545.4897</v>
       </c>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -4241,7 +4242,7 @@
         <v>3.199957862004851</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -4348,7 +4349,7 @@
         <v>61.951108538307679</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -4455,7 +4456,7 @@
         <v>73.3</v>
       </c>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -4562,7 +4563,7 @@
         <v>3909.4126647190683</v>
       </c>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>63</v>
       </c>
@@ -4669,7 +4670,7 @@
         <v>4441275649898.2539</v>
       </c>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>63</v>
       </c>
@@ -4776,7 +4777,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>63</v>
       </c>
@@ -4883,7 +4884,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>63</v>
       </c>
@@ -4990,7 +4991,7 @@
         <v>23852823.228</v>
       </c>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>63</v>
       </c>
@@ -5097,7 +5098,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>63</v>
       </c>
@@ -5204,7 +5205,7 @@
         <v>1136046775</v>
       </c>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>63</v>
       </c>
@@ -5311,7 +5312,7 @@
         <v>569076163</v>
       </c>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>63</v>
       </c>
@@ -5418,7 +5419,7 @@
         <v>2.6278240381451923</v>
       </c>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>63</v>
       </c>
@@ -5632,7 +5633,7 @@
         <v>1206.4480773137566</v>
       </c>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -5739,7 +5740,7 @@
         <v>11.545858256059923</v>
       </c>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -5846,7 +5847,7 @@
         <v>238333054798.785</v>
       </c>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -5953,7 +5954,7 @@
         <v>22605296107568.367</v>
       </c>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -6060,7 +6061,7 @@
         <v>-3.5485866054493158</v>
       </c>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -6167,7 +6168,7 @@
         <v>62025.976549731487</v>
       </c>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>43</v>
       </c>
@@ -6274,7 +6275,7 @@
         <v>62347.154206237479</v>
       </c>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>43</v>
       </c>
@@ -6381,7 +6382,7 @@
         <v>23043644547851.621</v>
       </c>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -6488,7 +6489,7 @@
         <v>0.74968046356758578</v>
       </c>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>43</v>
       </c>
@@ -6595,7 +6596,7 @@
         <v>77.74116293638761</v>
       </c>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>43</v>
       </c>
@@ -6702,7 +6703,7 @@
         <v>6.2</v>
       </c>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>43</v>
       </c>
@@ -6809,7 +6810,7 @@
         <v>61497.658690129967</v>
       </c>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>43</v>
       </c>
@@ -6916,7 +6917,7 @@
         <v>22729669147251.59</v>
       </c>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>43</v>
       </c>
@@ -7023,7 +7024,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -7130,7 +7131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="58" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>43</v>
       </c>
@@ -7237,7 +7238,7 @@
         <v>18113064</v>
       </c>
     </row>
-    <row r="59" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>43</v>
       </c>
@@ -7344,7 +7345,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="60" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>43</v>
       </c>
@@ -7451,7 +7452,7 @@
         <v>369602187</v>
       </c>
     </row>
-    <row r="61" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>43</v>
       </c>
@@ -7558,7 +7559,7 @@
         <v>186627018</v>
       </c>
     </row>
-    <row r="62" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>43</v>
       </c>
@@ -7665,7 +7666,7 @@
         <v>0.98555719446034118</v>
       </c>
     </row>
-    <row r="63" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>43</v>
       </c>
@@ -7879,7 +7880,7 @@
         <v>51368.378417676453</v>
       </c>
     </row>
-    <row r="65" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -7986,7 +7987,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="66" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>119</v>
       </c>
@@ -8093,7 +8094,7 @@
         <v>66074471585.507904</v>
       </c>
     </row>
-    <row r="67" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>119</v>
       </c>
@@ -8200,7 +8201,7 @@
         <v>3035580428041.8135</v>
       </c>
     </row>
-    <row r="68" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>119</v>
       </c>
@@ -8307,7 +8308,7 @@
         <v>-3.9877425243290787</v>
       </c>
     </row>
-    <row r="69" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>119</v>
       </c>
@@ -8414,7 +8415,7 @@
         <v>6892.3571516341945</v>
       </c>
     </row>
-    <row r="70" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>119</v>
       </c>
@@ -8521,7 +8522,7 @@
         <v>15990.292681556282</v>
       </c>
     </row>
-    <row r="71" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>119</v>
       </c>
@@ -8628,7 +8629,7 @@
         <v>7428168459283.8105</v>
       </c>
     </row>
-    <row r="72" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>119</v>
       </c>
@@ -8735,7 +8736,7 @@
         <v>0.29774474840355225</v>
       </c>
     </row>
-    <row r="73" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>119</v>
       </c>
@@ -8842,7 +8843,7 @@
         <v>74.447733743888591</v>
       </c>
     </row>
-    <row r="74" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>119</v>
       </c>
@@ -8949,7 +8950,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="75" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>119</v>
       </c>
@@ -9056,7 +9057,7 @@
         <v>16011.387472760342</v>
       </c>
     </row>
-    <row r="76" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>119</v>
       </c>
@@ -9163,7 +9164,7 @@
         <v>7437967883584.3994</v>
       </c>
     </row>
-    <row r="77" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>119</v>
       </c>
@@ -9270,7 +9271,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="78" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>119</v>
       </c>
@@ -9377,7 +9378,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="79" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>119</v>
       </c>
@@ -9484,7 +9485,7 @@
         <v>11223349</v>
       </c>
     </row>
-    <row r="80" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>119</v>
       </c>
@@ -9591,7 +9592,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="81" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>119</v>
       </c>
@@ -9698,7 +9699,7 @@
         <v>464542370</v>
       </c>
     </row>
-    <row r="82" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>119</v>
       </c>
@@ -9805,7 +9806,7 @@
         <v>223868601</v>
       </c>
     </row>
-    <row r="83" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>119</v>
       </c>
@@ -9912,7 +9913,7 @@
         <v>1.7150670324577675</v>
       </c>
     </row>
-    <row r="84" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>119</v>
       </c>
@@ -10126,7 +10127,7 @@
         <v>5597.4072959027399</v>
       </c>
     </row>
-    <row r="86" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>153</v>
       </c>
@@ -10233,7 +10234,7 @@
         <v>42.177909014762548</v>
       </c>
     </row>
-    <row r="87" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>153</v>
       </c>
@@ -10340,7 +10341,7 @@
         <v>96490937546.238266</v>
       </c>
     </row>
-    <row r="88" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>153</v>
       </c>
@@ -10447,7 +10448,7 @@
         <v>22121578723066.828</v>
       </c>
     </row>
-    <row r="89" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>153</v>
       </c>
@@ -10554,7 +10555,7 @@
         <v>-5.5805828270023028</v>
       </c>
     </row>
-    <row r="90" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>153</v>
       </c>
@@ -10661,7 +10662,7 @@
         <v>24056.823734464822</v>
       </c>
     </row>
-    <row r="91" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>153</v>
       </c>
@@ -10768,7 +10769,7 @@
         <v>35593.264732355055</v>
       </c>
     </row>
-    <row r="92" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>153</v>
       </c>
@@ -10875,7 +10876,7 @@
         <v>32857662079721.844</v>
       </c>
     </row>
-    <row r="93" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>153</v>
       </c>
@@ -10982,7 +10983,7 @@
         <v>1.9822074731686143</v>
       </c>
     </row>
-    <row r="94" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>153</v>
       </c>
@@ -11089,7 +11090,7 @@
         <v>77.390449729670934</v>
       </c>
     </row>
-    <row r="95" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>153</v>
       </c>
@@ -11196,7 +11197,7 @@
         <v>7.6</v>
       </c>
     </row>
-    <row r="96" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>153</v>
       </c>
@@ -11303,7 +11304,7 @@
         <v>35828.03963259083</v>
       </c>
     </row>
-    <row r="97" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -11410,7 +11411,7 @@
         <v>33074392812200.43</v>
       </c>
     </row>
-    <row r="98" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>153</v>
       </c>
@@ -11517,7 +11518,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="99" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>153</v>
       </c>
@@ -11624,7 +11625,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="100" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>153</v>
       </c>
@@ -11731,7 +11732,7 @@
         <v>27447886.685999997</v>
       </c>
     </row>
-    <row r="101" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>153</v>
       </c>
@@ -11838,7 +11839,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="102" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>153</v>
       </c>
@@ -11945,7 +11946,7 @@
         <v>923142688</v>
       </c>
     </row>
-    <row r="103" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>153</v>
       </c>
@@ -12052,7 +12053,7 @@
         <v>474225863</v>
       </c>
     </row>
-    <row r="104" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>153</v>
       </c>
@@ -12159,7 +12160,7 @@
         <v>0.25358999747278688</v>
       </c>
     </row>
-    <row r="105" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>153</v>
       </c>
@@ -12373,7 +12374,7 @@
         <v>19404.258286549502</v>
       </c>
     </row>
-    <row r="107" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>33</v>
       </c>
@@ -12480,7 +12481,7 @@
         <v>25.860909014454126</v>
       </c>
     </row>
-    <row r="108" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>33</v>
       </c>
@@ -12587,7 +12588,7 @@
         <v>467928405074.97076</v>
       </c>
     </row>
-    <row r="109" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>33</v>
       </c>
@@ -12694,7 +12695,7 @@
         <v>52392675685741.234</v>
       </c>
     </row>
-    <row r="110" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>33</v>
       </c>
@@ -12801,7 +12802,7 @@
         <v>-4.4693313920777484</v>
       </c>
     </row>
-    <row r="111" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>33</v>
       </c>
@@ -12908,7 +12909,7 @@
         <v>38595.674864000503</v>
       </c>
     </row>
-    <row r="112" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>33</v>
       </c>
@@ -13015,7 +13016,7 @@
         <v>45007.398718949436</v>
       </c>
     </row>
-    <row r="113" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>33</v>
       </c>
@@ -13122,7 +13123,7 @@
         <v>61780918775273.883</v>
       </c>
     </row>
-    <row r="114" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>33</v>
       </c>
@@ -13229,7 +13230,7 @@
         <v>1.4330929916014483</v>
       </c>
     </row>
-    <row r="115" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>33</v>
       </c>
@@ -13336,7 +13337,7 @@
         <v>79.701853222831957</v>
       </c>
     </row>
-    <row r="116" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>33</v>
       </c>
@@ -13443,7 +13444,7 @@
         <v>6.7572589367420246</v>
       </c>
     </row>
-    <row r="117" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>33</v>
       </c>
@@ -13550,7 +13551,7 @@
         <v>44855.39104156784</v>
       </c>
     </row>
-    <row r="118" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>33</v>
       </c>
@@ -13657,7 +13658,7 @@
         <v>61572260327177.961</v>
       </c>
     </row>
-    <row r="119" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>33</v>
       </c>
@@ -13764,7 +13765,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="120" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>33</v>
       </c>
@@ -13871,7 +13872,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="121" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>33</v>
       </c>
@@ -13978,7 +13979,7 @@
         <v>35511888.358999997</v>
       </c>
     </row>
-    <row r="122" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>33</v>
       </c>
@@ -14085,7 +14086,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="123" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>33</v>
       </c>
@@ -14192,7 +14193,7 @@
         <v>1372683615</v>
       </c>
     </row>
-    <row r="124" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>33</v>
       </c>
@@ -14299,7 +14300,7 @@
         <v>697188809</v>
       </c>
     </row>
-    <row r="125" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>33</v>
       </c>
@@ -14406,7 +14407,7 @@
         <v>0.56977372889876676</v>
       </c>
     </row>
-    <row r="126" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>33</v>
       </c>
@@ -14620,7 +14621,7 @@
         <v>31250.158159711256</v>
       </c>
     </row>
-    <row r="128" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>151</v>
       </c>
@@ -14727,7 +14728,7 @@
         <v>25.092302734774929</v>
       </c>
     </row>
-    <row r="129" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>151</v>
       </c>
@@ -14834,7 +14835,7 @@
         <v>163721634903.82816</v>
       </c>
     </row>
-    <row r="130" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>151</v>
       </c>
@@ -14941,7 +14942,7 @@
         <v>4725519821856.6836</v>
       </c>
     </row>
-    <row r="131" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>151</v>
       </c>
@@ -15048,7 +15049,7 @@
         <v>-6.7224272862207499</v>
       </c>
     </row>
-    <row r="132" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>151</v>
       </c>
@@ -15155,7 +15156,7 @@
         <v>7611.8367501578223</v>
       </c>
     </row>
-    <row r="133" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>151</v>
       </c>
@@ -15262,7 +15263,7 @@
         <v>15150.1718906773</v>
       </c>
     </row>
-    <row r="134" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>151</v>
       </c>
@@ -15369,7 +15370,7 @@
         <v>9883445824506.3887</v>
       </c>
     </row>
-    <row r="135" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>151</v>
       </c>
@@ -15476,7 +15477,7 @@
         <v>2.4293592949220439</v>
       </c>
     </row>
-    <row r="136" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>151</v>
       </c>
@@ -15583,7 +15584,7 @@
         <v>75.762427569980971</v>
       </c>
     </row>
-    <row r="137" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -15690,7 +15691,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="138" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>151</v>
       </c>
@@ -15797,7 +15798,7 @@
         <v>15643.016693840933</v>
       </c>
     </row>
-    <row r="139" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>151</v>
       </c>
@@ -15904,7 +15905,7 @@
         <v>10204960652661.881</v>
       </c>
     </row>
-    <row r="140" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>151</v>
       </c>
@@ -16011,7 +16012,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="141" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>151</v>
       </c>
@@ -16118,7 +16119,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="142" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>151</v>
       </c>
@@ -16225,7 +16226,7 @@
         <v>20038977</v>
       </c>
     </row>
-    <row r="143" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>151</v>
       </c>
@@ -16332,7 +16333,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="144" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>151</v>
       </c>
@@ -16439,7 +16440,7 @@
         <v>652365260</v>
       </c>
     </row>
-    <row r="145" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>151</v>
       </c>
@@ -16546,7 +16547,7 @@
         <v>331335264</v>
       </c>
     </row>
-    <row r="146" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>151</v>
       </c>
@@ -16653,7 +16654,7 @@
         <v>0.91790043062263749</v>
       </c>
     </row>
-    <row r="147" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>151</v>
       </c>
@@ -16867,7 +16868,7 @@
         <v>5589.8830618485918</v>
       </c>
     </row>
-    <row r="149" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>145</v>
       </c>
@@ -16974,7 +16975,7 @@
         <v>22.380828625212416</v>
       </c>
     </row>
-    <row r="150" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>145</v>
       </c>
@@ -17081,7 +17082,7 @@
         <v>141089044867.97263</v>
       </c>
     </row>
-    <row r="151" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>145</v>
       </c>
@@ -17188,7 +17189,7 @@
         <v>7384772400818.0586</v>
       </c>
     </row>
-    <row r="152" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>145</v>
       </c>
@@ -17295,7 +17296,7 @@
         <v>-3.4158321331902926</v>
       </c>
     </row>
-    <row r="153" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>145</v>
       </c>
@@ -17402,7 +17403,7 @@
         <v>2217.1490291966129</v>
       </c>
     </row>
-    <row r="154" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>145</v>
       </c>
@@ -17509,7 +17510,7 @@
         <v>7053.8845972534691</v>
       </c>
     </row>
-    <row r="155" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>145</v>
       </c>
@@ -17616,7 +17617,7 @@
         <v>23493956169636.547</v>
       </c>
     </row>
-    <row r="156" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>145</v>
       </c>
@@ -17723,7 +17724,7 @@
         <v>3.4251643576987902</v>
       </c>
     </row>
-    <row r="157" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>145</v>
       </c>
@@ -17830,7 +17831,7 @@
         <v>69.282818455687632</v>
       </c>
     </row>
-    <row r="158" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>145</v>
       </c>
@@ -17937,7 +17938,7 @@
         <v>44.9</v>
       </c>
     </row>
-    <row r="159" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>145</v>
       </c>
@@ -18044,7 +18045,7 @@
         <v>7135.9980029631306</v>
       </c>
     </row>
-    <row r="160" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>145</v>
       </c>
@@ -18151,7 +18152,7 @@
         <v>23767446432779.43</v>
       </c>
     </row>
-    <row r="161" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>145</v>
       </c>
@@ -18258,7 +18259,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="162" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>145</v>
       </c>
@@ -18365,7 +18366,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="163" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>145</v>
       </c>
@@ -18472,7 +18473,7 @@
         <v>25599745</v>
       </c>
     </row>
-    <row r="164" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>145</v>
       </c>
@@ -18579,7 +18580,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="165" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>145</v>
       </c>
@@ -18686,7 +18687,7 @@
         <v>3330640847</v>
       </c>
     </row>
-    <row r="166" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>145</v>
       </c>
@@ -18793,7 +18794,7 @@
         <v>1635876047</v>
       </c>
     </row>
-    <row r="167" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>145</v>
       </c>
@@ -18900,7 +18901,7 @@
         <v>1.3765065996418144</v>
       </c>
     </row>
-    <row r="168" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>145</v>
       </c>
@@ -19114,7 +19115,7 @@
         <v>1905.9590438694427</v>
       </c>
     </row>
-    <row r="170" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>14</v>
       </c>
@@ -19221,7 +19222,7 @@
         <v>18.525617518474039</v>
       </c>
     </row>
-    <row r="171" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>14</v>
       </c>
@@ -19328,7 +19329,7 @@
         <v>12628105316.168085</v>
       </c>
     </row>
-    <row r="172" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>14</v>
       </c>
@@ -19435,7 +19436,7 @@
         <v>459729949563.42346</v>
       </c>
     </row>
-    <row r="173" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>14</v>
       </c>
@@ -19542,7 +19543,7 @@
         <v>0.62141410583198819</v>
       </c>
     </row>
-    <row r="174" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>14</v>
       </c>
@@ -19649,7 +19650,7 @@
         <v>668.81542350927668</v>
       </c>
     </row>
-    <row r="175" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>14</v>
       </c>
@@ -19756,7 +19757,7 @@
         <v>1992.4410640867484</v>
       </c>
     </row>
-    <row r="176" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>14</v>
       </c>
@@ -19863,7 +19864,7 @@
         <v>1325270251071.6738</v>
       </c>
     </row>
-    <row r="177" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>14</v>
       </c>
@@ -19970,7 +19971,7 @@
         <v>6.2571632639612886</v>
       </c>
     </row>
-    <row r="178" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>14</v>
       </c>
@@ -20077,7 +20078,7 @@
         <v>64.0537576786637</v>
       </c>
     </row>
-    <row r="179" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>14</v>
       </c>
@@ -20184,7 +20185,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="180" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>14</v>
       </c>
@@ -20291,7 +20292,7 @@
         <v>2056.894655978283</v>
       </c>
     </row>
-    <row r="181" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>14</v>
       </c>
@@ -20398,7 +20399,7 @@
         <v>1368141495520.6118</v>
       </c>
     </row>
-    <row r="182" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>14</v>
       </c>
@@ -20505,7 +20506,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="183" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>14</v>
       </c>
@@ -20612,7 +20613,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="184" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>14</v>
       </c>
@@ -20719,7 +20720,7 @@
         <v>14953572.228</v>
       </c>
     </row>
-    <row r="185" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>14</v>
       </c>
@@ -20826,7 +20827,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="186" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>14</v>
       </c>
@@ -20933,7 +20934,7 @@
         <v>665149035</v>
       </c>
     </row>
-    <row r="187" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>14</v>
       </c>
@@ -21040,7 +21041,7 @@
         <v>333577700</v>
       </c>
     </row>
-    <row r="188" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>14</v>
       </c>
@@ -21147,7 +21148,7 @@
         <v>2.6669223843099417</v>
       </c>
     </row>
-    <row r="189" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>14</v>
       </c>
@@ -21361,7 +21362,7 @@
         <v>575.83967357858319</v>
       </c>
     </row>
-    <row r="191" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>179</v>
       </c>
@@ -21468,7 +21469,7 @@
         <v>28.809441447529561</v>
       </c>
     </row>
-    <row r="192" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>179</v>
       </c>
@@ -21575,7 +21576,7 @@
         <v>723885017025.23511</v>
       </c>
     </row>
-    <row r="193" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>179</v>
       </c>
@@ -21682,7 +21683,7 @@
         <v>53461077013094.648</v>
       </c>
     </row>
-    <row r="194" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>179</v>
       </c>
@@ -21789,7 +21790,7 @@
         <v>-4.4877898733149237</v>
       </c>
     </row>
-    <row r="195" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>179</v>
       </c>
@@ -21896,7 +21897,7 @@
         <v>44475.6210116246</v>
       </c>
     </row>
-    <row r="196" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>179</v>
       </c>
@@ -22003,7 +22004,7 @@
         <v>51195.335659111166</v>
       </c>
     </row>
-    <row r="197" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>179</v>
       </c>
@@ -22110,7 +22111,7 @@
         <v>62296253484830.164</v>
       </c>
     </row>
-    <row r="198" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>179</v>
       </c>
@@ -22217,7 +22218,7 @@
         <v>1.2155087299536262</v>
       </c>
     </row>
-    <row r="199" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>179</v>
       </c>
@@ -22324,7 +22325,7 @@
         <v>80.307239331014898</v>
       </c>
     </row>
-    <row r="200" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>179</v>
       </c>
@@ -22431,7 +22432,7 @@
         <v>4.9000000000000004</v>
       </c>
     </row>
-    <row r="201" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>179</v>
       </c>
@@ -22538,7 +22539,7 @@
         <v>50887.443535542763</v>
       </c>
     </row>
-    <row r="202" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>179</v>
       </c>
@@ -22645,7 +22646,7 @@
         <v>61921599709659.805</v>
       </c>
     </row>
-    <row r="203" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>179</v>
       </c>
@@ -22752,7 +22753,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="204" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>179</v>
       </c>
@@ -22859,7 +22860,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="205" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>179</v>
       </c>
@@ -22966,7 +22967,7 @@
         <v>34946338.286000006</v>
       </c>
     </row>
-    <row r="206" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>179</v>
       </c>
@@ -23073,7 +23074,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="207" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>179</v>
       </c>
@@ -23180,7 +23181,7 @@
         <v>1216834555</v>
       </c>
     </row>
-    <row r="208" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>179</v>
       </c>
@@ -23287,7 +23288,7 @@
         <v>610072709</v>
       </c>
     </row>
-    <row r="209" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>179</v>
       </c>
@@ -23394,7 +23395,7 @@
         <v>0.49329019294093257</v>
       </c>
     </row>
-    <row r="210" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>179</v>
       </c>
@@ -23608,7 +23609,7 @@
         <v>35966.208891907809</v>
       </c>
     </row>
-    <row r="212" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>37</v>
       </c>
@@ -23715,7 +23716,7 @@
         <v>22.581884246611779</v>
       </c>
     </row>
-    <row r="213" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>37</v>
       </c>
@@ -23822,7 +23823,7 @@
         <v>490277569762.17212</v>
       </c>
     </row>
-    <row r="214" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>37</v>
       </c>
@@ -23929,7 +23930,7 @@
         <v>30535343464998.676</v>
       </c>
     </row>
-    <row r="215" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>37</v>
       </c>
@@ -24036,7 +24037,7 @@
         <v>-1.3796613048442197</v>
       </c>
     </row>
-    <row r="216" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>37</v>
       </c>
@@ -24143,7 +24144,7 @@
         <v>5317.700253594614</v>
       </c>
     </row>
-    <row r="217" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>37</v>
       </c>
@@ -24250,7 +24251,7 @@
         <v>11689.748632505889</v>
       </c>
     </row>
-    <row r="218" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>37</v>
       </c>
@@ -24357,7 +24358,7 @@
         <v>68421023568830.281</v>
       </c>
     </row>
-    <row r="219" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>37</v>
       </c>
@@ -24464,7 +24465,7 @@
         <v>2.5764745006724468</v>
       </c>
     </row>
-    <row r="220" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>37</v>
       </c>
@@ -24571,7 +24572,7 @@
         <v>72.167808267268626</v>
       </c>
     </row>
-    <row r="221" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>37</v>
       </c>
@@ -24678,7 +24679,7 @@
         <v>34.099169327714073</v>
       </c>
     </row>
-    <row r="222" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>37</v>
       </c>
@@ -24785,7 +24786,7 @@
         <v>11854.088163520997</v>
       </c>
     </row>
-    <row r="223" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>37</v>
       </c>
@@ -24892,7 +24893,7 @@
         <v>69382915845419.367</v>
       </c>
     </row>
-    <row r="224" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>37</v>
       </c>
@@ -24999,7 +25000,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="225" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>37</v>
       </c>
@@ -25106,7 +25107,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="226" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>37</v>
       </c>
@@ -25213,7 +25214,7 @@
         <v>79167322.200000003</v>
       </c>
     </row>
-    <row r="227" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>37</v>
       </c>
@@ -25320,7 +25321,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="228" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>37</v>
       </c>
@@ -25427,7 +25428,7 @@
         <v>5853079114</v>
       </c>
     </row>
-    <row r="229" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>37</v>
       </c>
@@ -25534,7 +25535,7 @@
         <v>2889934743</v>
       </c>
     </row>
-    <row r="230" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>37</v>
       </c>
@@ -25641,7 +25642,7 @@
         <v>0.98149447583197968</v>
       </c>
     </row>
-    <row r="231" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>37</v>
       </c>
@@ -25855,7 +25856,7 @@
         <v>4045.5433552968484</v>
       </c>
     </row>
-    <row r="233" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>54</v>
       </c>
@@ -25962,7 +25963,7 @@
         <v>26.466989053154162</v>
       </c>
     </row>
-    <row r="234" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>54</v>
       </c>
@@ -26069,7 +26070,7 @@
         <v>1227749358770.2754</v>
       </c>
     </row>
-    <row r="235" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>54</v>
       </c>
@@ -26176,7 +26177,7 @@
         <v>84746978784172.844</v>
       </c>
     </row>
-    <row r="236" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>54</v>
       </c>
@@ -26283,7 +26284,7 @@
         <v>-3.2936830403669859</v>
       </c>
     </row>
-    <row r="237" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>54</v>
       </c>
@@ -26390,7 +26391,7 @@
         <v>11077.473273964117</v>
       </c>
     </row>
-    <row r="238" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>54</v>
       </c>
@@ -26497,7 +26498,7 @@
         <v>17050.875596013993</v>
       </c>
     </row>
-    <row r="239" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>54</v>
       </c>
@@ -26604,7 +26605,7 @@
         <v>132374449619819.97</v>
       </c>
     </row>
-    <row r="240" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>54</v>
       </c>
@@ -26711,7 +26712,7 @@
         <v>1.792082195461262</v>
       </c>
     </row>
-    <row r="241" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>54</v>
       </c>
@@ -26818,7 +26819,7 @@
         <v>72.747303139606046</v>
       </c>
     </row>
-    <row r="242" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>54</v>
       </c>
@@ -26925,7 +26926,7 @@
         <v>36.6</v>
       </c>
     </row>
-    <row r="243" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>54</v>
       </c>
@@ -27032,7 +27033,7 @@
         <v>17131.00889310518</v>
       </c>
     </row>
-    <row r="244" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>54</v>
       </c>
@@ -27139,7 +27140,7 @@
         <v>132996564363367.03</v>
       </c>
     </row>
-    <row r="245" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>54</v>
       </c>
@@ -27246,7 +27247,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="246" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>54</v>
       </c>
@@ -27353,7 +27354,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="247" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>54</v>
       </c>
@@ -27460,7 +27461,7 @@
         <v>129949282.714</v>
       </c>
     </row>
-    <row r="248" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>54</v>
       </c>
@@ -27567,7 +27568,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="249" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>54</v>
       </c>
@@ -27674,7 +27675,7 @@
         <v>7763498647</v>
       </c>
     </row>
-    <row r="250" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>54</v>
       </c>
@@ -27781,7 +27782,7 @@
         <v>3848036163</v>
       </c>
     </row>
-    <row r="251" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>54</v>
       </c>
@@ -27888,7 +27889,7 @@
         <v>1.0419901903243982</v>
       </c>
     </row>
-    <row r="252" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>54</v>
       </c>
@@ -28102,7 +28103,7 @@
         <v>8767.3992123669777</v>
       </c>
     </row>
-    <row r="254" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>132</v>
       </c>
@@ -28209,7 +28210,7 @@
         <v>19.596708970146128</v>
       </c>
     </row>
-    <row r="255" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>132</v>
       </c>
@@ -28316,7 +28317,7 @@
         <v>21922780787.845547</v>
       </c>
     </row>
-    <row r="256" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>132</v>
       </c>
@@ -28423,7 +28424,7 @@
         <v>1113396635024.4697</v>
       </c>
     </row>
-    <row r="257" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>132</v>
       </c>
@@ -28530,7 +28531,7 @@
         <v>0.69147669616505425</v>
       </c>
     </row>
-    <row r="258" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>132</v>
       </c>
@@ -28637,7 +28638,7 @@
         <v>1061.826777964375</v>
       </c>
     </row>
-    <row r="259" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>132</v>
       </c>
@@ -28744,7 +28745,7 @@
         <v>3095.3960381411839</v>
       </c>
     </row>
-    <row r="260" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>132</v>
       </c>
@@ -28851,7 +28852,7 @@
         <v>3272239149436.3765</v>
       </c>
     </row>
-    <row r="261" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>132</v>
       </c>
@@ -28958,7 +28959,7 @@
         <v>4.2206488218284619</v>
       </c>
     </row>
-    <row r="262" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>132</v>
       </c>
@@ -29065,7 +29066,7 @@
         <v>65.628939941568817</v>
       </c>
     </row>
-    <row r="263" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>132</v>
       </c>
@@ -29172,7 +29173,7 @@
         <v>60.654624288248975</v>
       </c>
     </row>
-    <row r="264" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>132</v>
       </c>
@@ -29279,7 +29280,7 @@
         <v>3124.2579049540905</v>
       </c>
     </row>
-    <row r="265" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>132</v>
       </c>
@@ -29386,7 +29387,7 @@
         <v>3302749923937.3755</v>
       </c>
     </row>
-    <row r="266" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>132</v>
       </c>
@@ -29493,7 +29494,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="267" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>132</v>
       </c>
@@ -29600,7 +29601,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="268" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>132</v>
       </c>
@@ -29707,7 +29708,7 @@
         <v>20372993.228</v>
       </c>
     </row>
-    <row r="269" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>132</v>
       </c>
@@ -29814,7 +29815,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="270" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>132</v>
       </c>
@@ -29921,7 +29922,7 @@
         <v>1057131013</v>
       </c>
     </row>
-    <row r="271" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>132</v>
       </c>
@@ -30028,7 +30029,7 @@
         <v>531264330</v>
       </c>
     </row>
-    <row r="272" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>132</v>
       </c>
@@ -30135,7 +30136,7 @@
         <v>2.3271980754618227</v>
       </c>
     </row>
-    <row r="273" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>132</v>
       </c>
@@ -30349,7 +30350,7 @@
         <v>937.44427891351495</v>
       </c>
     </row>
-    <row r="275" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>171</v>
       </c>
@@ -30456,7 +30457,7 @@
         <v>26.558272156308721</v>
       </c>
     </row>
-    <row r="276" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>171</v>
       </c>
@@ -30563,7 +30564,7 @@
         <v>564357558035.16418</v>
       </c>
     </row>
-    <row r="277" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>171</v>
       </c>
@@ -30670,7 +30671,7 @@
         <v>27097404937164.801</v>
       </c>
     </row>
-    <row r="278" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>171</v>
       </c>
@@ -30777,7 +30778,7 @@
         <v>-0.13331868653655476</v>
       </c>
     </row>
-    <row r="279" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>171</v>
       </c>
@@ -30884,7 +30885,7 @@
         <v>11745.24381060104</v>
       </c>
     </row>
-    <row r="280" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>171</v>
       </c>
@@ -30991,7 +30992,7 @@
         <v>18454.131746046311</v>
       </c>
     </row>
-    <row r="281" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>171</v>
       </c>
@@ -31098,7 +31099,7 @@
         <v>43568672713585.805</v>
       </c>
     </row>
-    <row r="282" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>171</v>
       </c>
@@ -31205,7 +31206,7 @@
         <v>1.2419754729642705</v>
       </c>
     </row>
-    <row r="283" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>171</v>
       </c>
@@ -31312,7 +31313,7 @@
         <v>76.443449707529368</v>
       </c>
     </row>
-    <row r="284" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>171</v>
       </c>
@@ -31419,7 +31420,7 @@
         <v>13.8</v>
       </c>
     </row>
-    <row r="285" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>171</v>
       </c>
@@ -31526,7 +31527,7 @@
         <v>18540.657569695129</v>
       </c>
     </row>
-    <row r="286" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>171</v>
       </c>
@@ -31633,7 +31634,7 @@
         <v>43772952998548.898</v>
       </c>
     </row>
-    <row r="287" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>171</v>
       </c>
@@ -31740,7 +31741,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="288" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>171</v>
       </c>
@@ -31847,7 +31848,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="289" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>171</v>
       </c>
@@ -31954,7 +31955,7 @@
         <v>24502428.799999997</v>
       </c>
     </row>
-    <row r="290" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>171</v>
       </c>
@@ -32061,7 +32062,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="291" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>171</v>
       </c>
@@ -32168,7 +32169,7 @@
         <v>2360916965</v>
       </c>
     </row>
-    <row r="292" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>171</v>
       </c>
@@ -32275,7 +32276,7 @@
         <v>1164640503</v>
       </c>
     </row>
-    <row r="293" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>171</v>
       </c>
@@ -32382,7 +32383,7 @@
         <v>0.432094057970005</v>
       </c>
     </row>
-    <row r="294" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>171</v>
       </c>
@@ -32596,7 +32597,7 @@
         <v>8628.3538346435598</v>
       </c>
     </row>
-    <row r="296" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>93</v>
       </c>
@@ -32703,7 +32704,7 @@
         <v>22.620329535239122</v>
       </c>
     </row>
-    <row r="297" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>93</v>
       </c>
@@ -32810,7 +32811,7 @@
         <v>12913412761.475733</v>
       </c>
     </row>
-    <row r="298" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>93</v>
       </c>
@@ -32917,7 +32918,7 @@
         <v>920792331527.74561</v>
       </c>
     </row>
-    <row r="299" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>93</v>
       </c>
@@ -33024,7 +33025,7 @@
         <v>-2.9391855811121985</v>
       </c>
     </row>
-    <row r="300" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>93</v>
       </c>
@@ -33131,7 +33132,7 @@
         <v>1406.2890068375611</v>
       </c>
     </row>
-    <row r="301" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>93</v>
       </c>
@@ -33238,7 +33239,7 @@
         <v>3591.3725576203906</v>
       </c>
     </row>
-    <row r="302" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>93</v>
       </c>
@@ -33345,7 +33346,7 @@
         <v>2432232998860.9009</v>
       </c>
     </row>
-    <row r="303" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>93</v>
       </c>
@@ -33452,7 +33453,7 @@
         <v>5.3735891420049455</v>
       </c>
     </row>
-    <row r="304" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>93</v>
       </c>
@@ -33559,7 +33560,7 @@
         <v>64.325702231480349</v>
       </c>
     </row>
-    <row r="305" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>93</v>
       </c>
@@ -33666,7 +33667,7 @@
         <v>58.158649582168039</v>
       </c>
     </row>
-    <row r="306" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>93</v>
       </c>
@@ -33773,7 +33774,7 @@
         <v>3684.5626231375804</v>
       </c>
     </row>
-    <row r="307" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>93</v>
       </c>
@@ -33880,7 +33881,7 @@
         <v>2495345346265.7886</v>
       </c>
     </row>
-    <row r="308" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>93</v>
       </c>
@@ -33987,7 +33988,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="309" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>93</v>
       </c>
@@ -34094,7 +34095,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="310" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>93</v>
       </c>
@@ -34201,7 +34202,7 @@
         <v>14807043.228</v>
       </c>
     </row>
-    <row r="311" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>93</v>
       </c>
@@ -34308,7 +34309,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="312" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>93</v>
       </c>
@@ -34415,7 +34416,7 @@
         <v>677243299</v>
       </c>
     </row>
-    <row r="313" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>93</v>
       </c>
@@ -34522,7 +34523,7 @@
         <v>341090736</v>
       </c>
     </row>
-    <row r="314" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>93</v>
       </c>
@@ -34629,7 +34630,7 @@
         <v>2.60542748736259</v>
       </c>
     </row>
-    <row r="315" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>93</v>
       </c>
@@ -34843,7 +34844,7 @@
         <v>1089.3321435383486</v>
       </c>
     </row>
-    <row r="317" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>162</v>
       </c>
@@ -34950,7 +34951,7 @@
         <v>22.654815245430903</v>
       </c>
     </row>
-    <row r="318" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>162</v>
       </c>
@@ -35057,7 +35058,7 @@
         <v>349188524894.19952</v>
       </c>
     </row>
-    <row r="319" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>162</v>
       </c>
@@ -35164,7 +35165,7 @@
         <v>23150665555175.715</v>
       </c>
     </row>
-    <row r="320" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>162</v>
       </c>
@@ -35271,7 +35272,7 @@
         <v>-0.71323166478546796</v>
       </c>
     </row>
-    <row r="321" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>162</v>
       </c>
@@ -35378,7 +35379,7 @@
         <v>9412.2801953336166</v>
       </c>
     </row>
-    <row r="322" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>162</v>
       </c>
@@ -35485,7 +35486,7 @@
         <v>17800.293008616783</v>
       </c>
     </row>
-    <row r="323" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>162</v>
       </c>
@@ -35592,7 +35593,7 @@
         <v>44900140248747.539</v>
       </c>
     </row>
-    <row r="324" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>162</v>
       </c>
@@ -35699,7 +35700,7 @@
         <v>1.3569255643566365</v>
       </c>
     </row>
-    <row r="325" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>162</v>
       </c>
@@ -35806,7 +35807,7 @@
         <v>75.977463397364389</v>
       </c>
     </row>
-    <row r="326" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>162</v>
       </c>
@@ -35913,7 +35914,7 @@
         <v>11.2</v>
       </c>
     </row>
-    <row r="327" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>162</v>
       </c>
@@ -36020,7 +36021,7 @@
         <v>18073.148150746318</v>
       </c>
     </row>
-    <row r="328" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>162</v>
       </c>
@@ -36127,7 +36128,7 @@
         <v>45588400500602.797</v>
       </c>
     </row>
-    <row r="329" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>162</v>
       </c>
@@ -36234,7 +36235,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="330" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>162</v>
       </c>
@@ -36341,7 +36342,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="331" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>162</v>
       </c>
@@ -36448,7 +36449,7 @@
         <v>53567577.200000003</v>
       </c>
     </row>
-    <row r="332" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A332" t="s">
         <v>162</v>
       </c>
@@ -36555,7 +36556,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="333" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A333" t="s">
         <v>162</v>
       </c>
@@ -36662,7 +36663,7 @@
         <v>2522438267</v>
       </c>
     </row>
-    <row r="334" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A334" t="s">
         <v>162</v>
       </c>
@@ -36769,7 +36770,7 @@
         <v>1254058696</v>
       </c>
     </row>
-    <row r="335" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A335" t="s">
         <v>162</v>
       </c>
@@ -36876,7 +36877,7 @@
         <v>0.46461002915276595</v>
       </c>
     </row>
-    <row r="336" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:35" hidden="1" x14ac:dyDescent="0.3">
       <c r="A336" t="s">
         <v>162</v>
       </c>
@@ -37107,7 +37108,13 @@
       <c r="D341" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AI1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:AI337" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Adjusted net national income per capita (current US$)"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>